<commit_message>
Mise à jour des remarque fait sur le dossier rendu sur la première partie stat descriptive
</commit_message>
<xml_diff>
--- a/Script/données_complètes_9_classes_MEFG_stagiaire_tatistique.xlsx
+++ b/Script/données_complètes_9_classes_MEFG_stagiaire_tatistique.xlsx
@@ -864,7 +864,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2429" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2429" uniqueCount="1041">
   <si>
     <t>classe</t>
   </si>
@@ -3945,9 +3945,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cadres et professions intellectuelles supérieures </t>
-  </si>
-  <si>
-    <t>Infirmier</t>
   </si>
   <si>
     <t>Ouvrier</t>
@@ -4584,8 +4581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BA1" sqref="BA1:BA1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AU131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BC153" sqref="BC153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -4607,7 +4604,7 @@
   <sheetData>
     <row r="1" spans="1:55" s="6" customFormat="1">
       <c r="A1" s="42" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>0</v>
@@ -4622,10 +4619,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>1030</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>1031</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>4</v>
@@ -4933,7 +4930,7 @@
         <v>1012</v>
       </c>
       <c r="BB2" s="30" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC2" s="30" t="s">
         <v>1024</v>
@@ -5270,7 +5267,7 @@
         <v>1024</v>
       </c>
       <c r="BC4" s="33" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="5" spans="1:55" s="31" customFormat="1" ht="28.8">
@@ -5601,7 +5598,7 @@
         <v>1012</v>
       </c>
       <c r="BB6" s="33" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC6" s="34" t="s">
         <v>1022</v>
@@ -5768,7 +5765,7 @@
         <v>1012</v>
       </c>
       <c r="BB7" s="30" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="BC7" s="35" t="s">
         <v>1022</v>
@@ -5935,7 +5932,7 @@
         <v>1012</v>
       </c>
       <c r="BB8" s="33" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC8" s="34"/>
     </row>
@@ -6267,7 +6264,7 @@
         <v>1012</v>
       </c>
       <c r="BB10" s="33" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="BC10" s="33" t="s">
         <v>1021</v>
@@ -6764,7 +6761,7 @@
         <v>1012</v>
       </c>
       <c r="BB13" s="33" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC13" s="34" t="s">
         <v>1022</v>
@@ -7597,7 +7594,7 @@
         <v>1012</v>
       </c>
       <c r="BB18" s="21" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="BC18" s="21" t="s">
         <v>1024</v>
@@ -8435,7 +8432,7 @@
         <v>1022</v>
       </c>
       <c r="BC23" s="21" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="24" spans="1:55">
@@ -9264,10 +9261,10 @@
         <v>99.5</v>
       </c>
       <c r="BA28" s="20" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="BB28" s="23" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="BC28" s="23" t="s">
         <v>1024</v>
@@ -9431,7 +9428,7 @@
         <v>99.5</v>
       </c>
       <c r="BA29" s="20" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="BB29" s="21" t="s">
         <v>1024</v>
@@ -9596,7 +9593,7 @@
         <v>99.5</v>
       </c>
       <c r="BA30" s="20" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="BB30" s="21" t="s">
         <v>1024</v>
@@ -11434,10 +11431,10 @@
         <v>1012</v>
       </c>
       <c r="BB41" s="36" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC41" s="36" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="42" spans="1:55" s="31" customFormat="1">
@@ -11604,7 +11601,7 @@
         <v>1024</v>
       </c>
       <c r="BC42" s="36" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="43" spans="1:55" s="31" customFormat="1" ht="28.8">
@@ -13274,7 +13271,7 @@
         <v>1025</v>
       </c>
       <c r="BC52" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="53" spans="1:55" ht="28.8">
@@ -13772,10 +13769,10 @@
         <v>1012</v>
       </c>
       <c r="BB55" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC55" s="21" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="56" spans="1:55" ht="28.8">
@@ -13942,7 +13939,7 @@
         <v>1023</v>
       </c>
       <c r="BC56" s="23" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="57" spans="1:55">
@@ -14276,7 +14273,7 @@
         <v>1021</v>
       </c>
       <c r="BC58" s="21" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="59" spans="1:55" ht="28.8">
@@ -14443,7 +14440,7 @@
         <v>1023</v>
       </c>
       <c r="BC59" s="21" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="60" spans="1:55" ht="28.8">
@@ -15111,7 +15108,7 @@
         <v>1023</v>
       </c>
       <c r="BC63" s="21" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="64" spans="1:55" ht="28.8">
@@ -15612,7 +15609,7 @@
         <v>1024</v>
       </c>
       <c r="BC66" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="67" spans="1:55" s="31" customFormat="1" ht="28.8">
@@ -17936,7 +17933,7 @@
         <v>1024</v>
       </c>
       <c r="BC80" s="36" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="81" spans="1:55" s="31" customFormat="1" ht="28.8">
@@ -18766,7 +18763,7 @@
         <v>1012</v>
       </c>
       <c r="BB85" s="36" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="BC85" s="36" t="s">
         <v>1024</v>
@@ -18936,7 +18933,7 @@
         <v>1024</v>
       </c>
       <c r="BC86" s="36" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="87" spans="1:55" s="31" customFormat="1" ht="28.8">
@@ -19600,7 +19597,7 @@
         <v>1025</v>
       </c>
       <c r="BC90" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="91" spans="1:55">
@@ -20929,7 +20926,7 @@
         <v>1012</v>
       </c>
       <c r="BB98" s="22" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="BC98" s="22"/>
     </row>
@@ -22088,7 +22085,7 @@
         <v>1012</v>
       </c>
       <c r="BB105" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC105" s="22"/>
     </row>
@@ -22420,10 +22417,10 @@
         <v>1012</v>
       </c>
       <c r="BB107" s="21" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="BC107" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="108" spans="1:55">
@@ -22587,10 +22584,10 @@
         <v>1012</v>
       </c>
       <c r="BB108" s="21" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="BC108" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="109" spans="1:55" s="31" customFormat="1">
@@ -22927,7 +22924,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="111" spans="1:55" s="31" customFormat="1">
+    <row r="111" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A111" s="28" t="s">
         <v>595</v>
       </c>
@@ -23091,7 +23088,7 @@
         <v>1025</v>
       </c>
       <c r="BC111" s="40" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="112" spans="1:55" s="31" customFormat="1" ht="28.8">
@@ -23422,7 +23419,7 @@
         <v>1012</v>
       </c>
       <c r="BB113" s="40" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC113" s="40"/>
     </row>
@@ -24751,7 +24748,7 @@
         <v>1024</v>
       </c>
       <c r="BC121" s="40" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="122" spans="1:55" s="31" customFormat="1">
@@ -25252,7 +25249,7 @@
         <v>1021</v>
       </c>
       <c r="BC124" s="40" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="125" spans="1:55" s="31" customFormat="1">
@@ -25747,7 +25744,7 @@
         <v>86.1</v>
       </c>
       <c r="BA127" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB127" s="21" t="s">
         <v>1023</v>
@@ -25914,13 +25911,13 @@
         <v>86.1</v>
       </c>
       <c r="BA128" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB128" s="21" t="s">
         <v>1025</v>
       </c>
       <c r="BC128" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="129" spans="1:55">
@@ -26081,10 +26078,10 @@
         <v>86.1</v>
       </c>
       <c r="BA129" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB129" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC129" s="21" t="s">
         <v>1024</v>
@@ -26248,7 +26245,7 @@
         <v>86.1</v>
       </c>
       <c r="BA130" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB130" s="21" t="s">
         <v>1024</v>
@@ -26415,10 +26412,10 @@
         <v>86.1</v>
       </c>
       <c r="BA131" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB131" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC131" s="22"/>
     </row>
@@ -26580,7 +26577,7 @@
         <v>86.1</v>
       </c>
       <c r="BA132" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB132" s="21" t="s">
         <v>1021</v>
@@ -26747,7 +26744,7 @@
         <v>86.1</v>
       </c>
       <c r="BA133" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB133" s="21" t="s">
         <v>1024</v>
@@ -26914,7 +26911,7 @@
         <v>86.1</v>
       </c>
       <c r="BA134" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB134" s="21"/>
       <c r="BC134" s="22"/>
@@ -27077,7 +27074,7 @@
         <v>86.1</v>
       </c>
       <c r="BA135" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB135" s="21" t="s">
         <v>1025</v>
@@ -27244,10 +27241,10 @@
         <v>86.1</v>
       </c>
       <c r="BA136" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB136" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC136" s="21" t="s">
         <v>1024</v>
@@ -27411,7 +27408,7 @@
         <v>86.1</v>
       </c>
       <c r="BA137" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB137" s="21" t="s">
         <v>1021</v>
@@ -27578,7 +27575,7 @@
         <v>86.1</v>
       </c>
       <c r="BA138" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB138" s="21" t="s">
         <v>1023</v>
@@ -27745,7 +27742,7 @@
         <v>86.1</v>
       </c>
       <c r="BA139" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB139" s="21" t="s">
         <v>1024</v>
@@ -27912,7 +27909,7 @@
         <v>86.1</v>
       </c>
       <c r="BA140" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB140" s="21" t="s">
         <v>1024</v>
@@ -28079,7 +28076,7 @@
         <v>86.1</v>
       </c>
       <c r="BA141" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB141" s="21" t="s">
         <v>1021</v>
@@ -28244,7 +28241,7 @@
         <v>86.1</v>
       </c>
       <c r="BA142" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB142" s="21" t="s">
         <v>1023</v>
@@ -28411,7 +28408,7 @@
         <v>86.1</v>
       </c>
       <c r="BA143" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB143" s="21" t="s">
         <v>1021</v>
@@ -28578,10 +28575,10 @@
         <v>86.1</v>
       </c>
       <c r="BA144" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB144" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC144" s="22"/>
     </row>
@@ -28743,10 +28740,10 @@
         <v>86.1</v>
       </c>
       <c r="BA145" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB145" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC145" s="21" t="s">
         <v>1024</v>
@@ -28910,7 +28907,7 @@
         <v>86.1</v>
       </c>
       <c r="BA146" s="13" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="BB146" s="21" t="s">
         <v>1021</v>
@@ -29083,7 +29080,7 @@
         <v>1021</v>
       </c>
       <c r="BC147" s="36" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="148" spans="1:55" s="31" customFormat="1" ht="28.8">
@@ -30081,7 +30078,7 @@
         <v>1023</v>
       </c>
       <c r="BC153" s="37" t="s">
-        <v>1027</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="154" spans="1:55" s="31" customFormat="1">
@@ -30248,7 +30245,7 @@
         <v>1021</v>
       </c>
       <c r="BC154" s="36" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="155" spans="1:55" s="31" customFormat="1">
@@ -30574,7 +30571,7 @@
       </c>
       <c r="BB156" s="37"/>
       <c r="BC156" s="36" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="157" spans="1:55" s="31" customFormat="1">
@@ -31071,7 +31068,7 @@
         <v>1021</v>
       </c>
       <c r="BC159" s="36" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="160" spans="1:55" s="31" customFormat="1">
@@ -31238,7 +31235,7 @@
         <v>1021</v>
       </c>
       <c r="BC160" s="36" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="161" spans="1:55" s="31" customFormat="1" ht="28.8">
@@ -31569,7 +31566,7 @@
         <v>1012</v>
       </c>
       <c r="BB162" s="37" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="BC162" s="36" t="s">
         <v>1025</v>

</xml_diff>